<commit_message>
Prio créa de map
</commit_message>
<xml_diff>
--- a/Docs/Prio.xlsx
+++ b/Docs/Prio.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projets\C Party\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Couch_Party\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Unifier le vocabulaire des fonctionnalités</t>
   </si>
@@ -120,13 +120,23 @@
   </si>
   <si>
     <t>Ne pas oublier de faire remonter les Bugs</t>
+  </si>
+  <si>
+    <t>Création de la map</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,13 +198,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,24 +520,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44EEBBA7-D4A5-48E4-B590-45E9065EBDB3}">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.5703125" customWidth="1"/>
-    <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="1" max="1" width="51.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14" style="3" customWidth="1"/>
+    <col min="3" max="4" width="11.42578125" style="3"/>
+    <col min="5" max="5" width="20" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="4"/>
+      <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -536,7 +549,7 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="4">
         <v>0</v>
       </c>
     </row>
@@ -544,7 +557,7 @@
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="4">
         <v>0</v>
       </c>
     </row>
@@ -552,7 +565,7 @@
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="4">
         <v>0</v>
       </c>
     </row>
@@ -560,7 +573,7 @@
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="4">
         <v>0</v>
       </c>
     </row>
@@ -568,7 +581,7 @@
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="4">
         <v>0</v>
       </c>
     </row>
@@ -576,7 +589,7 @@
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="4">
         <v>0</v>
       </c>
     </row>
@@ -584,7 +597,7 @@
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="4">
         <v>0</v>
       </c>
     </row>
@@ -592,7 +605,7 @@
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="4">
         <v>0</v>
       </c>
     </row>
@@ -600,7 +613,7 @@
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="4">
         <v>0</v>
       </c>
     </row>
@@ -608,7 +621,7 @@
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="4"/>
+      <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
@@ -618,7 +631,7 @@
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="5">
         <v>1</v>
       </c>
     </row>
@@ -626,7 +639,7 @@
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="4">
         <v>0</v>
       </c>
     </row>
@@ -634,7 +647,7 @@
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="4">
         <v>0</v>
       </c>
     </row>
@@ -642,7 +655,7 @@
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="4">
         <v>0</v>
       </c>
     </row>
@@ -650,7 +663,7 @@
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="4">
         <v>0</v>
       </c>
     </row>
@@ -658,7 +671,7 @@
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="4">
         <v>0</v>
       </c>
     </row>
@@ -666,7 +679,7 @@
       <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="4"/>
+      <c r="B22" s="2"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
@@ -676,7 +689,7 @@
       <c r="A24" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="4">
         <v>0</v>
       </c>
     </row>
@@ -684,7 +697,7 @@
       <c r="A26" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="4"/>
+      <c r="B26" s="2"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
@@ -694,7 +707,7 @@
       <c r="A28" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="4">
         <v>0</v>
       </c>
     </row>
@@ -702,7 +715,7 @@
       <c r="A29" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="4">
         <v>0</v>
       </c>
     </row>
@@ -710,7 +723,7 @@
       <c r="A30" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30" s="4">
         <v>0</v>
       </c>
     </row>
@@ -718,7 +731,7 @@
       <c r="A31" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="4">
         <v>0</v>
       </c>
     </row>
@@ -726,7 +739,7 @@
       <c r="A33" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B33" s="4"/>
+      <c r="B33" s="2"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
@@ -736,7 +749,7 @@
       <c r="A35" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -744,7 +757,7 @@
       <c r="A36" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36" s="4">
         <v>0</v>
       </c>
     </row>
@@ -752,7 +765,7 @@
       <c r="A37" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B37" s="4">
         <v>0</v>
       </c>
     </row>
@@ -778,7 +791,16 @@
       </c>
       <c r="B42" s="1"/>
     </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" s="4">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mise en place de l'input manager à 100%
</commit_message>
<xml_diff>
--- a/Docs/Prio.xlsx
+++ b/Docs/Prio.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Couch_P\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jordan\Couch_Party\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
   <si>
     <t>Unifier le vocabulaire des fonctionnalités</t>
   </si>
@@ -118,9 +118,6 @@
   </si>
   <si>
     <t>Mécaniques de Grab Objects</t>
-  </si>
-  <si>
-    <t>(A pauffiner)</t>
   </si>
   <si>
     <t>Ui Déplacements</t>
@@ -261,9 +258,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -589,7 +586,7 @@
   <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,7 +605,7 @@
       </c>
       <c r="B1" s="2"/>
       <c r="D1" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -628,10 +625,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>31</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -666,14 +660,14 @@
         <v>0.8</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>0</v>
       </c>
     </row>
@@ -681,7 +675,7 @@
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="6">
         <v>0</v>
       </c>
     </row>
@@ -697,15 +691,15 @@
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="7">
         <v>0.4</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="6">
+        <v>35</v>
+      </c>
+      <c r="B13" s="5">
         <v>0</v>
       </c>
     </row>
@@ -774,7 +768,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="4">
         <v>1</v>
@@ -782,7 +776,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" s="4">
         <v>1</v>
@@ -790,7 +784,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" s="4">
         <v>1</v>
@@ -798,7 +792,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26" s="4">
         <v>1</v>
@@ -806,7 +800,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B27" s="4">
         <v>1</v>
@@ -814,9 +808,9 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" s="7">
+        <v>42</v>
+      </c>
+      <c r="B28" s="6">
         <v>0</v>
       </c>
     </row>
@@ -864,40 +858,40 @@
       <c r="A37" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B37" s="5">
+      <c r="B37" s="7">
         <v>0.5</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B38" s="5">
+      <c r="B38" s="7">
         <v>0.5</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B39" s="5">
+        <v>37</v>
+      </c>
+      <c r="B39" s="7">
         <v>0.25</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B40" s="7">
+        <v>41</v>
+      </c>
+      <c r="B40" s="6">
         <v>0</v>
       </c>
     </row>
@@ -927,7 +921,7 @@
       <c r="A45" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B45" s="6">
+      <c r="B45" s="5">
         <v>0</v>
       </c>
     </row>
@@ -935,7 +929,7 @@
       <c r="A46" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B46" s="5">
+      <c r="B46" s="7">
         <v>0.3</v>
       </c>
     </row>
@@ -943,7 +937,7 @@
       <c r="A47" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B47" s="5">
+      <c r="B47" s="7">
         <v>0.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
intégration des sons dans le menu principal
</commit_message>
<xml_diff>
--- a/Docs/Prio.xlsx
+++ b/Docs/Prio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\OneDrive\Documents\Couch_Party\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="032D89BC67406262B7FC6EF0CC60CD7E2FCF2F1F" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{E21004B1-00A8-4304-A973-A68067F0B542}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="032D89BC67406262B7FC6EF0CC60CD7E2FCF2F1F" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{71F5E545-DB86-4CBE-B23B-E37EADB84349}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12216" xr2:uid="{ACCB3BAB-0A22-414B-8B50-5F6751B2C8D8}"/>
   </bookViews>
@@ -250,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -269,6 +269,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44EEBBA7-D4A5-48E4-B590-45E9065EBDB3}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -633,7 +634,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="4">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -810,8 +811,8 @@
       <c r="A28" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="6">
-        <v>0</v>
+      <c r="B28" s="18">
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Sons pour 3 2 1 + Klaxon bateau
</commit_message>
<xml_diff>
--- a/Docs/Prio.xlsx
+++ b/Docs/Prio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\OneDrive\Documents\Couch_Party\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="032D89BC67406262B7FC6EF0CC60CD7E2FCF2F1F" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{71F5E545-DB86-4CBE-B23B-E37EADB84349}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="032D89BC67406262B7FC6EF0CC60CD7E2FCF2F1F" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{0AC46487-1BD8-4031-A0EC-70BF071CE01D}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12216" xr2:uid="{ACCB3BAB-0A22-414B-8B50-5F6751B2C8D8}"/>
   </bookViews>
@@ -586,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44EEBBA7-D4A5-48E4-B590-45E9065EBDB3}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>